<commit_message>
Added Automation Test Suite
</commit_message>
<xml_diff>
--- a/Interview_Task.xlsx
+++ b/Interview_Task.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\InterviewProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA6F212-600F-4661-81D4-59AF9EB09FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D99B1C-9730-4B2D-AFE0-E0763C9F0EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9454" yWindow="1414" windowWidth="23126" windowHeight="12043" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="3360" windowWidth="23126" windowHeight="12043" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenario" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="129">
   <si>
     <t>E-Commerce Test_Scenarios</t>
   </si>
@@ -486,6 +486,10 @@
   <si>
     <t>User should signout from account</t>
   </si>
+  <si>
+    <t>1. User should be login successfully
+2. user should see User name as UI design</t>
+  </si>
 </sst>
 </file>
 
@@ -798,6 +802,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -823,18 +839,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1095,32 +1099,32 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="27"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="31"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="30"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="34"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
@@ -1153,7 +1157,7 @@
       <c r="C6" s="8">
         <v>1</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="35" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="9" t="s">
@@ -1176,7 +1180,7 @@
       <c r="C7" s="8">
         <v>2</v>
       </c>
-      <c r="D7" s="32"/>
+      <c r="D7" s="36"/>
       <c r="E7" s="10" t="s">
         <v>9</v>
       </c>
@@ -1197,7 +1201,7 @@
       <c r="C8" s="8">
         <v>3</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="10" t="s">
         <v>10</v>
       </c>
@@ -1218,7 +1222,7 @@
       <c r="C9" s="8">
         <v>4</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="10" t="s">
         <v>11</v>
       </c>
@@ -1237,7 +1241,7 @@
       <c r="C10" s="8">
         <v>5</v>
       </c>
-      <c r="D10" s="32"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="10" t="s">
         <v>12</v>
       </c>
@@ -1256,7 +1260,7 @@
       <c r="C11" s="8">
         <v>6</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="36"/>
       <c r="E11" s="10" t="s">
         <v>13</v>
       </c>
@@ -1275,7 +1279,7 @@
       <c r="C12" s="8">
         <v>7</v>
       </c>
-      <c r="D12" s="32"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="9" t="s">
         <v>14</v>
       </c>
@@ -1294,7 +1298,7 @@
       <c r="C13" s="8">
         <v>8</v>
       </c>
-      <c r="D13" s="32"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="9" t="s">
         <v>15</v>
       </c>
@@ -1312,7 +1316,7 @@
       <c r="C14" s="8">
         <v>9</v>
       </c>
-      <c r="D14" s="32"/>
+      <c r="D14" s="36"/>
       <c r="E14" s="9" t="s">
         <v>16</v>
       </c>
@@ -1331,7 +1335,7 @@
       <c r="C15" s="8">
         <v>10</v>
       </c>
-      <c r="D15" s="33"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="10" t="s">
         <v>17</v>
       </c>
@@ -14240,14 +14244,14 @@
       <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
@@ -14305,20 +14309,20 @@
       <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="38" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
@@ -14745,7 +14749,7 @@
       <c r="B54" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="40" t="s">
+      <c r="C54" s="25" t="s">
         <v>32</v>
       </c>
     </row>
@@ -14778,7 +14782,7 @@
       <c r="B57" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="41" t="s">
+      <c r="C57" s="26" t="s">
         <v>36</v>
       </c>
     </row>
@@ -14800,7 +14804,7 @@
       <c r="B59" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C59" s="41" t="s">
+      <c r="C59" s="26" t="s">
         <v>40</v>
       </c>
     </row>
@@ -14808,32 +14812,32 @@
       <c r="A60" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="B60" s="42" t="s">
+      <c r="B60" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="C60" s="41" t="s">
+      <c r="C60" s="26" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.45" x14ac:dyDescent="0.3">
-      <c r="A61" s="43" t="s">
+      <c r="A61" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="B61" s="42" t="s">
+      <c r="B61" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="C61" s="41" t="s">
+      <c r="C61" s="26" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A62" s="43" t="s">
+      <c r="A62" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="B62" s="42" t="s">
+      <c r="B62" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="C62" s="41" t="s">
+      <c r="C62" s="26" t="s">
         <v>127</v>
       </c>
     </row>
@@ -14896,25 +14900,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="27"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="31"/>
       <c r="AD2" s="24"/>
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="30"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="13" t="s">
@@ -14942,24 +14946,24 @@
       </c>
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="34" t="s">
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="38" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="15" t="s">
@@ -15233,7 +15237,7 @@
       <c r="D37" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="40" t="s">
+      <c r="E37" s="25" t="s">
         <v>32</v>
       </c>
     </row>
@@ -15266,7 +15270,7 @@
       <c r="D40" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E40" s="41" t="s">
+      <c r="E40" s="26" t="s">
         <v>36</v>
       </c>
     </row>
@@ -15288,40 +15292,40 @@
       <c r="D42" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="41" t="s">
+      <c r="E42" s="26" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="43" t="s">
+      <c r="C43" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="42" t="s">
+      <c r="D43" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="E43" s="41" t="s">
+      <c r="E43" s="26" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="44" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="43" t="s">
+      <c r="C44" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="42" t="s">
+      <c r="D44" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="E44" s="41" t="s">
+      <c r="E44" s="26" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="45" spans="3:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="43" t="s">
+      <c r="C45" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="42" t="s">
+      <c r="D45" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="E45" s="41" t="s">
+      <c r="E45" s="26" t="s">
         <v>127</v>
       </c>
     </row>
@@ -15344,10 +15348,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD26"/>
+  <dimension ref="A1:AD29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -15365,70 +15369,70 @@
       <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="41"/>
+      <c r="AD3" s="41"/>
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="36"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="36"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="40"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="13" t="s">
@@ -15456,26 +15460,26 @@
       </c>
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
-      <c r="B15" s="34" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="38" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
@@ -15615,8 +15619,58 @@
       </c>
       <c r="E26" s="2"/>
     </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
@@ -15629,23 +15683,6 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="E15:E16"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>